<commit_message>
I commit this version cause it works but have to redo multithreaded
</commit_message>
<xml_diff>
--- a/Waves/comparison.xlsx
+++ b/Waves/comparison.xlsx
@@ -225,22 +225,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.1000000000000001E-2</c:v>
+                  <c:v>2.9350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0999999999999999E-2</c:v>
+                  <c:v>1.23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8000000000000001E-2</c:v>
+                  <c:v>2.6339999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1000000000000002E-2</c:v>
+                  <c:v>3.5259999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9000000000000002E-2</c:v>
+                  <c:v>9.1180000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11899999999999999</c:v>
+                  <c:v>7.5490000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -343,8 +343,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="365071968"/>
-        <c:axId val="365079584"/>
+        <c:axId val="-40193312"/>
+        <c:axId val="-40191680"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -488,7 +488,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365071968"/>
+        <c:axId val="-40193312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365079584"/>
+        <c:crossAx val="-40191680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -600,7 +600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365079584"/>
+        <c:axId val="-40191680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365071968"/>
+        <c:crossAx val="-40193312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,22 +938,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>3.9929999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>2.3380000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>3.153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4E-2</c:v>
+                  <c:v>7.4080000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>7.1219999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2999999999999999E-2</c:v>
+                  <c:v>8.7070000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1029,8 +1029,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="365081216"/>
-        <c:axId val="365081760"/>
+        <c:axId val="-40190048"/>
+        <c:axId val="-172439344"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1163,7 +1163,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$8:$B$13</c15:sqref>
@@ -1196,7 +1196,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$8:$C$13</c15:sqref>
@@ -1234,7 +1234,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365081216"/>
+        <c:axId val="-40190048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365081760"/>
+        <c:crossAx val="-172439344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1341,7 +1341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365081760"/>
+        <c:axId val="-172439344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365081216"/>
+        <c:crossAx val="-40190048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1674,22 +1674,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.02</c:v>
+                  <c:v>4.6950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>2.1429999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02</c:v>
+                  <c:v>2.3839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>2.7789999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4E-2</c:v>
+                  <c:v>5.2640000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>6.718</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1792,8 +1792,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361636656"/>
-        <c:axId val="361633936"/>
+        <c:axId val="-172443696"/>
+        <c:axId val="-2007881664"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1897,7 +1897,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361636656"/>
+        <c:axId val="-172443696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +1996,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361633936"/>
+        <c:crossAx val="-2007881664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2004,7 +2004,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361633936"/>
+        <c:axId val="-2007881664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,7 +2116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361636656"/>
+        <c:crossAx val="-172443696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4211,7 +4211,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4247,7 +4247,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="D2">
-        <v>2.1000000000000001E-2</v>
+        <v>2.9350000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="D3">
-        <v>1.0999999999999999E-2</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,7 +4275,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D4">
-        <v>2.8000000000000001E-2</v>
+        <v>2.6339999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
         <v>16.728000000000002</v>
       </c>
       <c r="D5">
-        <v>4.1000000000000002E-2</v>
+        <v>3.5259999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4303,7 +4303,7 @@
         <v>56.326000000000001</v>
       </c>
       <c r="D6">
-        <v>4.9000000000000002E-2</v>
+        <v>9.1180000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4317,7 +4317,7 @@
         <v>122.241</v>
       </c>
       <c r="D7">
-        <v>0.11899999999999999</v>
+        <v>7.5490000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,7 +4331,7 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="D8">
-        <v>1.7000000000000001E-2</v>
+        <v>3.9929999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4345,7 +4345,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D9">
-        <v>3.0000000000000001E-3</v>
+        <v>2.3380000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4359,7 +4359,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="D10">
-        <v>7.0000000000000001E-3</v>
+        <v>3.153</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4373,7 +4373,7 @@
         <v>34.933999999999997</v>
       </c>
       <c r="D11">
-        <v>1.4E-2</v>
+        <v>7.4080000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4387,7 +4387,7 @@
         <v>168.501</v>
       </c>
       <c r="D12">
-        <v>2.9000000000000001E-2</v>
+        <v>7.1219999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>476.64800000000002</v>
       </c>
       <c r="D13">
-        <v>5.2999999999999999E-2</v>
+        <v>8.7070000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="D14">
-        <v>0.02</v>
+        <v>4.6950000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4429,7 +4429,7 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="D15">
-        <v>1.4999999999999999E-2</v>
+        <v>2.1429999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="D16">
-        <v>0.02</v>
+        <v>2.3839999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4457,7 +4457,7 @@
         <v>22.872</v>
       </c>
       <c r="D17">
-        <v>3.1E-2</v>
+        <v>2.7789999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4471,7 +4471,7 @@
         <v>116.645</v>
       </c>
       <c r="D18">
-        <v>1.4E-2</v>
+        <v>5.2640000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4485,7 +4485,7 @@
         <v>328.29500000000002</v>
       </c>
       <c r="D19">
-        <v>3.2000000000000001E-2</v>
+        <v>6.718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updated version for multithreaded
</commit_message>
<xml_diff>
--- a/Waves/comparison.xlsx
+++ b/Waves/comparison.xlsx
@@ -225,22 +225,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.9350000000000001</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.23</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6339999999999999</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5259999999999998</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1180000000000003</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5490000000000004</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -343,8 +343,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-40193312"/>
-        <c:axId val="-40191680"/>
+        <c:axId val="-809702480"/>
+        <c:axId val="-809704656"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -488,7 +488,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-40193312"/>
+        <c:axId val="-809702480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-40191680"/>
+        <c:crossAx val="-809704656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -600,7 +600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-40191680"/>
+        <c:axId val="-809704656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-40193312"/>
+        <c:crossAx val="-809702480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,22 +938,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.9929999999999999</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3380000000000001</c:v>
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.153</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4080000000000004</c:v>
+                  <c:v>1.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1219999999999999</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.7070000000000007</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1029,8 +1029,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-40190048"/>
-        <c:axId val="-172439344"/>
+        <c:axId val="-630509312"/>
+        <c:axId val="-630503872"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1234,7 +1234,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-40190048"/>
+        <c:axId val="-630509312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,7 +1333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-172439344"/>
+        <c:crossAx val="-630503872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1341,7 +1341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-172439344"/>
+        <c:axId val="-630503872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-40190048"/>
+        <c:crossAx val="-630509312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1674,22 +1674,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.6950000000000003</c:v>
+                  <c:v>0.38700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1429999999999998</c:v>
+                  <c:v>0.13400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3839999999999999</c:v>
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7789999999999999</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2640000000000002</c:v>
+                  <c:v>4.9000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.718</c:v>
+                  <c:v>3.9E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1792,8 +1792,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-172443696"/>
-        <c:axId val="-2007881664"/>
+        <c:axId val="-630496800"/>
+        <c:axId val="-630497344"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1897,7 +1897,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-172443696"/>
+        <c:axId val="-630496800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +1996,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2007881664"/>
+        <c:crossAx val="-630497344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2004,7 +2004,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2007881664"/>
+        <c:axId val="-630497344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,7 +2116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-172443696"/>
+        <c:crossAx val="-630496800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4211,7 +4211,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4247,7 +4247,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="D2">
-        <v>2.9350000000000001</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="D3">
-        <v>1.23</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,7 +4275,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D4">
-        <v>2.6339999999999999</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
         <v>16.728000000000002</v>
       </c>
       <c r="D5">
-        <v>3.5259999999999998</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4303,7 +4303,7 @@
         <v>56.326000000000001</v>
       </c>
       <c r="D6">
-        <v>9.1180000000000003</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4317,7 +4317,7 @@
         <v>122.241</v>
       </c>
       <c r="D7">
-        <v>7.5490000000000004</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,7 +4331,7 @@
         <v>0.17899999999999999</v>
       </c>
       <c r="D8">
-        <v>3.9929999999999999</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4345,7 +4345,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D9">
-        <v>2.3380000000000001</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4359,7 +4359,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="D10">
-        <v>3.153</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4373,7 +4373,7 @@
         <v>34.933999999999997</v>
       </c>
       <c r="D11">
-        <v>7.4080000000000004</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4387,7 +4387,7 @@
         <v>168.501</v>
       </c>
       <c r="D12">
-        <v>7.1219999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>476.64800000000002</v>
       </c>
       <c r="D13">
-        <v>8.7070000000000007</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="D14">
-        <v>4.6950000000000003</v>
+        <v>0.38700000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4429,7 +4429,7 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="D15">
-        <v>2.1429999999999998</v>
+        <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="D16">
-        <v>2.3839999999999999</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4457,7 +4457,7 @@
         <v>22.872</v>
       </c>
       <c r="D17">
-        <v>2.7789999999999999</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4471,7 +4471,7 @@
         <v>116.645</v>
       </c>
       <c r="D18">
-        <v>5.2640000000000002</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4485,7 +4485,7 @@
         <v>328.29500000000002</v>
       </c>
       <c r="D19">
-        <v>6.718</v>
+        <v>3.9E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>